<commit_message>
fehler in der beschriftung der methoden verbessert
</commit_message>
<xml_diff>
--- a/data/molekueleModellieren_remondaten.xlsx
+++ b/data/molekueleModellieren_remondaten.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="70">
   <si>
     <t>Moleküle Modellieren</t>
   </si>
@@ -29,18 +29,6 @@
     <t>Aufgabe 1: Ethan</t>
   </si>
   <si>
-    <t>ZIND01</t>
-  </si>
-  <si>
-    <t>ZINDOS</t>
-  </si>
-  <si>
-    <t>TNDO</t>
-  </si>
-  <si>
-    <t>ab-initio minimal</t>
-  </si>
-  <si>
     <t>Semiempirisch</t>
   </si>
   <si>
@@ -98,9 +86,6 @@
     <t>Aufgabe 2: Tetrachlorethan</t>
   </si>
   <si>
-    <t>MNDO</t>
-  </si>
-  <si>
     <t>AM1</t>
   </si>
   <si>
@@ -243,13 +228,16 @@
   </si>
   <si>
     <t>-587.472106933594</t>
+  </si>
+  <si>
+    <t>wir hätten aufjedenfall werte rausnotieren sollen dafür aber ich kann mich beim besten willen ned dran erinnern dass er das je erwähnt hat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +268,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4B4B4B"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -468,7 +462,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
@@ -480,6 +473,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -501,8 +497,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,7 +574,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ZIND01</c:v>
+                  <c:v>AM1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -757,7 +751,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ZINDOS</c:v>
+                  <c:v>RM1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -934,7 +928,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TNDO</c:v>
+                  <c:v>PM3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1111,7 +1105,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ab-initio minimal</c:v>
+                  <c:v>Ab-Initio(Small)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1620,7 +1614,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MNDO</c:v>
+                  <c:v>RM1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1797,7 +1791,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AM1</c:v>
+                  <c:v>PM3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3767,8 +3761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47:D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3783,28 +3777,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="3" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="29"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
+      <c r="B5" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3812,30 +3806,30 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
-      <c r="C7" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
+      <c r="C7" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
       <c r="F7" s="8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3846,13 +3840,13 @@
         <v>-670.62890625</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3863,13 +3857,13 @@
         <v>-670.95343017578102</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3880,13 +3874,13 @@
         <v>-671.59429931640602</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3897,13 +3891,13 @@
         <v>-671.91082763671898</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3914,13 +3908,13 @@
         <v>-671.59429931640602</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3931,13 +3925,13 @@
         <v>-670.95343017578102</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3948,13 +3942,13 @@
         <v>-670.62890625</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3965,13 +3959,13 @@
         <v>-670.95343017578102</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -3982,13 +3976,13 @@
         <v>-671.59429931640602</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -3999,13 +3993,13 @@
         <v>-671.91082763671898</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -4016,13 +4010,13 @@
         <v>-671.59429931640602</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -4033,13 +4027,13 @@
         <v>-670.95343017578102</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -4050,13 +4044,13 @@
         <v>-670.62890625</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -4067,13 +4061,13 @@
         <v>-670.95343017578102</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -4084,13 +4078,13 @@
         <v>-671.59429931640602</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -4101,13 +4095,13 @@
         <v>-671.91082763671898</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -4118,13 +4112,13 @@
         <v>-671.59429931640602</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
@@ -4135,13 +4129,13 @@
         <v>-670.95343017578102</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
@@ -4152,61 +4146,61 @@
         <v>-670.62890625</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
+      <c r="B29" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="14" t="s">
+      <c r="I31" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>17</v>
-      </c>
       <c r="J31" s="13"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="4">
+      <c r="B32" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="1">
         <v>-7821.0050000000001</v>
       </c>
       <c r="D32" s="1">
         <v>46.607999999999997</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="1">
         <v>-7819.7560000000003</v>
       </c>
       <c r="F32" s="1">
@@ -4226,16 +4220,16 @@
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="4">
+      <c r="B33" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="1">
         <v>-7763.1360000000004</v>
       </c>
       <c r="D33" s="1">
         <v>45.194000000000003</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="1">
         <v>-7761.7449999999999</v>
       </c>
       <c r="F33" s="1">
@@ -4255,16 +4249,16 @@
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34">
+      <c r="B34" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="1">
         <v>-7611.6329999999998</v>
       </c>
       <c r="D34" s="1">
         <v>46.475999999999999</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="1">
         <v>-7610.2039999999997</v>
       </c>
       <c r="F34" s="1">
@@ -4284,30 +4278,30 @@
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="16">
+      <c r="B35" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="1">
         <v>-49443.951999999997</v>
       </c>
-      <c r="D35" s="16">
+      <c r="D35" s="1">
         <v>50.23</v>
       </c>
-      <c r="E35" s="16">
+      <c r="E35" s="1">
         <v>-49440.146999999997</v>
       </c>
-      <c r="F35" s="16">
+      <c r="F35" s="1">
         <v>49.844999999999999</v>
       </c>
-      <c r="G35" s="17">
+      <c r="G35" s="16">
         <f t="shared" si="0"/>
         <v>3.805000000000291</v>
       </c>
-      <c r="H35" s="17">
+      <c r="H35" s="16">
         <f t="shared" si="1"/>
         <v>-0.38499999999999801</v>
       </c>
-      <c r="I35" s="17">
+      <c r="I35" s="16">
         <f t="shared" si="2"/>
         <v>3.420000000000293</v>
       </c>
@@ -4343,21 +4337,21 @@
       </c>
     </row>
     <row r="39" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="18"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18">
+      <c r="B39" s="17"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G40">
         <f>AVERAGE(G32:G39)</f>
@@ -4371,15 +4365,15 @@
         <f>AVERAGE(I32:I39)</f>
         <v>0.72150000000008863</v>
       </c>
-      <c r="K40" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="L40" s="26"/>
-      <c r="M40" s="26"/>
+      <c r="K40" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G41">
         <f>_xlfn.STDEV.S(G32:G39)</f>
@@ -4396,7 +4390,7 @@
     </row>
     <row r="42" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -4416,320 +4410,320 @@
       </c>
     </row>
     <row r="44" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B44" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="27"/>
+      <c r="B44" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="29"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
-      <c r="C46" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="29"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="23"/>
+      <c r="C46" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="31"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="22"/>
     </row>
     <row r="47" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" t="s">
-        <v>28</v>
-      </c>
-      <c r="D47" t="s">
-        <v>29</v>
-      </c>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
+        <v>4</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
         <v>0</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
+        <v>39</v>
+      </c>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>20</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
+        <v>41</v>
+      </c>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="1">
         <v>40</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
+        <v>43</v>
+      </c>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
     </row>
     <row r="51" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" s="1">
         <v>60</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
+        <v>45</v>
+      </c>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
     </row>
     <row r="52" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <v>80</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
+        <v>47</v>
+      </c>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
         <v>100</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
+        <v>49</v>
+      </c>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="1">
         <v>120</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
+        <v>51</v>
+      </c>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
         <v>140</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E55" s="21"/>
-      <c r="F55" s="21"/>
+        <v>53</v>
+      </c>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="1">
         <v>160</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
+        <v>55</v>
+      </c>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
         <v>180</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
+        <v>57</v>
+      </c>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="1">
         <v>200</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
+        <v>55</v>
+      </c>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="1">
         <v>220</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
+        <v>60</v>
+      </c>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="1">
         <v>240</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E60" s="21"/>
-      <c r="F60" s="21"/>
+        <v>62</v>
+      </c>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="1">
         <v>260</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E61" s="21"/>
-      <c r="F61" s="21"/>
+        <v>49</v>
+      </c>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="1">
         <v>280</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
+        <v>47</v>
+      </c>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="1">
         <v>300</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E63" s="21"/>
-      <c r="F63" s="21"/>
+        <v>45</v>
+      </c>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="1">
         <v>320</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E64" s="21"/>
-      <c r="F64" s="21"/>
+        <v>43</v>
+      </c>
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="1">
         <v>340</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E65" s="21"/>
-      <c r="F65" s="21"/>
+        <v>68</v>
+      </c>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="1">
         <v>360</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
+        <v>39</v>
+      </c>
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
     </row>
     <row r="71" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G71" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H71" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D71" s="14" t="s">
+      <c r="I71" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E71" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F71" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G71" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H71" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I71" s="14" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B72" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C72" s="4">
+      <c r="B72" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C72" s="1">
         <v>-41867.949000000001</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D72" s="1">
         <v>22.440999999999999</v>
       </c>
-      <c r="E72" s="4">
+      <c r="E72" s="1">
         <v>-41857.142</v>
       </c>
-      <c r="F72" s="4">
+      <c r="F72" s="1">
         <v>22.181999999999999</v>
       </c>
       <c r="G72">
@@ -4746,16 +4740,16 @@
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C73" s="4">
+      <c r="B73" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" s="1">
         <v>-35400.07</v>
       </c>
       <c r="D73" s="1">
         <v>23.074000000000002</v>
       </c>
-      <c r="E73" s="4">
+      <c r="E73" s="1">
         <v>-35393.39</v>
       </c>
       <c r="F73" s="1">
@@ -4781,18 +4775,18 @@
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="18"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="20"/>
-      <c r="G75" s="18"/>
-      <c r="H75" s="18"/>
-      <c r="I75" s="18"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
     </row>
     <row r="76" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G76">
         <f>AVERAGE(G68:G75)</f>
@@ -4809,7 +4803,7 @@
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G77">
         <f>_xlfn.STDEV.S(G68:G75)</f>
@@ -4826,7 +4820,7 @@
     </row>
     <row r="78" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
@@ -4864,10 +4858,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C30" sqref="C30:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4878,38 +4872,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="A1" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
-      <c r="C3" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="C3" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -5164,7 +5158,7 @@
         <v>2.16015625</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
         <v>240</v>
       </c>
@@ -5185,7 +5179,7 @@
         <v>2.8828125</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
         <v>260</v>
       </c>
@@ -5206,7 +5200,7 @@
         <v>2.16015625</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
         <v>280</v>
       </c>
@@ -5227,7 +5221,7 @@
         <v>0.71875</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
         <v>300</v>
       </c>
@@ -5248,7 +5242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
         <v>320</v>
       </c>
@@ -5269,7 +5263,7 @@
         <v>0.71875</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
         <v>340</v>
       </c>
@@ -5290,11 +5284,11 @@
         <v>2.16015625</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="12">
         <v>360</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23">
         <f>Eingabe!C27-Eingabe!$C$12</f>
         <v>1.2819213867189774</v>
       </c>
@@ -5311,273 +5305,278 @@
         <v>2.8828125</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A27" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="27"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A27" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="29"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="C29" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="29"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="31"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="24">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="23">
         <v>0</v>
       </c>
-      <c r="C31" s="25">
+      <c r="C31" s="24">
         <f>Eingabe!C48-Eingabe!$C$51</f>
         <v>10.272033691406023</v>
       </c>
-      <c r="D31" s="21">
+      <c r="D31" s="20">
         <f>Eingabe!D48-Eingabe!$D$51</f>
         <v>6.1387329101560226</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="24">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="23">
         <v>20</v>
       </c>
-      <c r="C32" s="25">
+      <c r="C32" s="24">
         <f>Eingabe!C49-Eingabe!$C$51</f>
         <v>7.6693115234379547</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="20">
         <f>Eingabe!D49-Eingabe!$D$51</f>
         <v>4.033447265625</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="24">
+      <c r="B33" s="23">
         <v>40</v>
       </c>
-      <c r="C33" s="25">
+      <c r="C33" s="24">
         <f>Eingabe!C50-Eingabe!$C$51</f>
         <v>2.7266845703129547</v>
       </c>
-      <c r="D33" s="21">
+      <c r="D33" s="20">
         <f>Eingabe!D50-Eingabe!$D$51</f>
         <v>1.0166015625</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="24">
+      <c r="B34" s="23">
         <v>60</v>
       </c>
-      <c r="C34" s="25">
+      <c r="C34" s="24">
         <f>Eingabe!C51-Eingabe!$C$51</f>
         <v>0</v>
       </c>
-      <c r="D34" s="21">
+      <c r="D34" s="20">
         <f>Eingabe!D51-Eingabe!$D$51</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="24">
+      <c r="B35" s="23">
         <v>80</v>
       </c>
-      <c r="C35" s="25">
+      <c r="C35" s="24">
         <f>Eingabe!C52-Eingabe!$C$51</f>
         <v>0.67401123046897737</v>
       </c>
-      <c r="D35" s="21">
+      <c r="D35" s="20">
         <f>Eingabe!D52-Eingabe!$D$51</f>
         <v>0.40563964843704525</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="24">
+      <c r="B36" s="23">
         <v>100</v>
       </c>
-      <c r="C36" s="25">
+      <c r="C36" s="24">
         <f>Eingabe!C53-Eingabe!$C$51</f>
         <v>2.6248168945310226</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="20">
         <f>Eingabe!D53-Eingabe!$D$51</f>
         <v>1.943115234375</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="24">
+      <c r="B37" s="23">
         <v>120</v>
       </c>
-      <c r="C37" s="25">
+      <c r="C37" s="24">
         <f>Eingabe!C54-Eingabe!$C$51</f>
         <v>3.0176391601560226</v>
       </c>
-      <c r="D37" s="21">
+      <c r="D37" s="20">
         <f>Eingabe!D54-Eingabe!$D$51</f>
         <v>2.7783813476560226</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="24">
+      <c r="B38" s="23">
         <v>140</v>
       </c>
-      <c r="C38" s="25">
+      <c r="C38" s="24">
         <f>Eingabe!C55-Eingabe!$C$51</f>
         <v>0.89892578125</v>
       </c>
-      <c r="D38" s="21">
+      <c r="D38" s="20">
         <f>Eingabe!D55-Eingabe!$D$51</f>
         <v>1.3999633789060226</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="24">
+      <c r="B39" s="23">
         <v>160</v>
       </c>
-      <c r="C39" s="25">
+      <c r="C39" s="24">
         <f>Eingabe!C56-Eingabe!$C$51</f>
         <v>-1.7510986328120453</v>
       </c>
-      <c r="D39" s="21">
+      <c r="D39" s="20">
         <f>Eingabe!D56-Eingabe!$D$51</f>
         <v>-0.17742919921897737</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="24">
+      <c r="B40" s="23">
         <v>180</v>
       </c>
-      <c r="C40" s="25">
+      <c r="C40" s="24">
         <f>Eingabe!C57-Eingabe!$C$51</f>
         <v>-2.7799682617189774</v>
       </c>
-      <c r="D40" s="21">
+      <c r="D40" s="20">
         <f>Eingabe!D57-Eingabe!$D$51</f>
         <v>-0.61370849609397737</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="24">
+      <c r="B41" s="23">
         <v>200</v>
       </c>
-      <c r="C41" s="25">
+      <c r="C41" s="24">
         <f>Eingabe!C58-Eingabe!$C$51</f>
         <v>-1.7510375976560226</v>
       </c>
-      <c r="D41" s="21">
+      <c r="D41" s="20">
         <f>Eingabe!D58-Eingabe!$D$51</f>
         <v>-0.17742919921897737</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="24">
+      <c r="B42" s="23">
         <v>220</v>
       </c>
-      <c r="C42" s="25">
+      <c r="C42" s="24">
         <f>Eingabe!C59-Eingabe!$C$51</f>
         <v>0.89910888671897737</v>
       </c>
-      <c r="D42" s="21">
+      <c r="D42" s="20">
         <f>Eingabe!D59-Eingabe!$D$51</f>
         <v>1.4000244140620453</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="24">
+      <c r="B43" s="23">
         <v>240</v>
       </c>
-      <c r="C43" s="25">
+      <c r="C43" s="24">
         <f>Eingabe!C60-Eingabe!$C$51</f>
         <v>3.017822265625</v>
       </c>
-      <c r="D43" s="21">
+      <c r="D43" s="20">
         <f>Eingabe!D60-Eingabe!$D$51</f>
         <v>2.7784423828120453</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="24">
+      <c r="B44" s="23">
         <v>260</v>
       </c>
-      <c r="C44" s="25">
+      <c r="C44" s="24">
         <f>Eingabe!C61-Eingabe!$C$51</f>
         <v>2.625</v>
       </c>
-      <c r="D44" s="21">
+      <c r="D44" s="20">
         <f>Eingabe!D61-Eingabe!$D$51</f>
         <v>1.943115234375</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="24">
+      <c r="B45" s="23">
         <v>280</v>
       </c>
-      <c r="C45" s="25">
+      <c r="C45" s="24">
         <f>Eingabe!C62-Eingabe!$C$51</f>
         <v>0.67413330078102263</v>
       </c>
-      <c r="D45" s="21">
+      <c r="D45" s="20">
         <f>Eingabe!D62-Eingabe!$D$51</f>
         <v>0.40563964843704525</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="24">
+      <c r="B46" s="23">
         <v>300</v>
       </c>
-      <c r="C46" s="25">
+      <c r="C46" s="24">
         <f>Eingabe!C63-Eingabe!$C$51</f>
         <v>6.1035156022626325E-5</v>
       </c>
-      <c r="D46" s="21">
+      <c r="D46" s="20">
         <f>Eingabe!D63-Eingabe!$D$51</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="24">
+      <c r="B47" s="23">
         <v>320</v>
       </c>
-      <c r="C47" s="25">
+      <c r="C47" s="24">
         <f>Eingabe!C64-Eingabe!$C$51</f>
         <v>2.7267456054689774</v>
       </c>
-      <c r="D47" s="21">
+      <c r="D47" s="20">
         <f>Eingabe!D64-Eingabe!$D$51</f>
         <v>1.0166015625</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="24">
+      <c r="B48" s="23">
         <v>340</v>
       </c>
-      <c r="C48" s="25">
+      <c r="C48" s="24">
         <f>Eingabe!C65-Eingabe!$C$51</f>
         <v>7.6694946289060226</v>
       </c>
-      <c r="D48" s="21">
+      <c r="D48" s="20">
         <f>Eingabe!D65-Eingabe!$D$51</f>
         <v>4.0335083007810226</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="24">
+      <c r="B49" s="23">
         <v>360</v>
       </c>
-      <c r="C49" s="25">
+      <c r="C49" s="24">
         <f>Eingabe!C66-Eingabe!$C$51</f>
         <v>10.272033691406023</v>
       </c>
-      <c r="D49" s="21">
+      <c r="D49" s="20">
         <f>Eingabe!D66-Eingabe!$D$51</f>
         <v>6.1387329101560226</v>
       </c>

</xml_diff>